<commit_message>
updated data after refactoring for rds efficiencies
</commit_message>
<xml_diff>
--- a/output/county_grandtots_bothyears_11daysout.xlsx
+++ b/output/county_grandtots_bothyears_11daysout.xlsx
@@ -7435,7 +7435,7 @@
         <v>36632</v>
       </c>
       <c r="L162">
-        <v>82.48999999999999</v>
+        <v>82.49</v>
       </c>
     </row>
     <row r="163">
@@ -8323,7 +8323,7 @@
         <v>8368</v>
       </c>
       <c r="L186">
-        <v>67.12</v>
+        <v>67.12000000000001</v>
       </c>
     </row>
     <row r="187">
@@ -25425,7 +25425,7 @@
         <v>3791</v>
       </c>
       <c r="L572">
-        <v>71.98999999999999</v>
+        <v>71.99</v>
       </c>
     </row>
     <row r="573">
@@ -26989,7 +26989,7 @@
         <v>604</v>
       </c>
       <c r="L606">
-        <v>64.73999999999999</v>
+        <v>64.74</v>
       </c>
     </row>
     <row r="607">
@@ -27081,7 +27081,7 @@
         <v>9231</v>
       </c>
       <c r="L608">
-        <v>67.48999999999999</v>
+        <v>67.49</v>
       </c>
     </row>
     <row r="609">
@@ -33199,7 +33199,7 @@
         <v>25888</v>
       </c>
       <c r="L777">
-        <v>98.87</v>
+        <v>98.87000000000001</v>
       </c>
     </row>
     <row r="778">
@@ -38811,7 +38811,7 @@
         <v>128</v>
       </c>
       <c r="L899">
-        <v>86.48999999999999</v>
+        <v>86.49</v>
       </c>
     </row>
     <row r="900">
@@ -41626,7 +41626,7 @@
         <v>3465</v>
       </c>
       <c r="L969">
-        <v>84.48999999999999</v>
+        <v>84.49</v>
       </c>
     </row>
     <row r="970">
@@ -50170,7 +50170,7 @@
         <v>1227</v>
       </c>
       <c r="L1170">
-        <v>604.4299999999999</v>
+        <v>604.43</v>
       </c>
     </row>
     <row r="1171">
@@ -51095,7 +51095,7 @@
         <v>955</v>
       </c>
       <c r="L1195">
-        <v>624.1799999999999</v>
+        <v>624.18</v>
       </c>
     </row>
     <row r="1196">
@@ -52816,7 +52816,7 @@
         <v>60</v>
       </c>
       <c r="L1233">
-        <v>95.23999999999999</v>
+        <v>95.24</v>
       </c>
     </row>
     <row r="1234">
@@ -53092,7 +53092,7 @@
         <v>7168</v>
       </c>
       <c r="L1239">
-        <v>93.37</v>
+        <v>93.37000000000001</v>
       </c>
     </row>
     <row r="1240">
@@ -53552,7 +53552,7 @@
         <v>547</v>
       </c>
       <c r="L1249">
-        <v>98.73999999999999</v>
+        <v>98.74</v>
       </c>
     </row>
     <row r="1250">
@@ -56588,7 +56588,7 @@
         <v>1184</v>
       </c>
       <c r="L1315">
-        <v>538.1799999999999</v>
+        <v>538.18</v>
       </c>
     </row>
     <row r="1316">
@@ -56910,7 +56910,7 @@
         <v>223</v>
       </c>
       <c r="L1322">
-        <v>81.98999999999999</v>
+        <v>81.99</v>
       </c>
     </row>
     <row r="1323">
@@ -59072,7 +59072,7 @@
         <v>26968</v>
       </c>
       <c r="L1369">
-        <v>609.3099999999999</v>
+        <v>609.31</v>
       </c>
     </row>
     <row r="1370">
@@ -60774,7 +60774,7 @@
         <v>1009</v>
       </c>
       <c r="L1406">
-        <v>85.87</v>
+        <v>85.87000000000001</v>
       </c>
     </row>
     <row r="1407">
@@ -66644,7 +66644,7 @@
         <v>278</v>
       </c>
       <c r="L1534">
-        <v>84.23999999999999</v>
+        <v>84.24</v>
       </c>
     </row>
     <row r="1535">
@@ -69864,7 +69864,7 @@
         <v>1856</v>
       </c>
       <c r="L1604">
-        <v>77.37</v>
+        <v>77.37000000000001</v>
       </c>
     </row>
     <row r="1605">
@@ -70692,7 +70692,7 @@
         <v>4824</v>
       </c>
       <c r="L1622">
-        <v>83.12</v>
+        <v>83.12000000000001</v>
       </c>
     </row>
     <row r="1623">
@@ -87746,7 +87746,7 @@
         <v>797</v>
       </c>
       <c r="L2090">
-        <v>8855.559999999999</v>
+        <v>8855.56</v>
       </c>
     </row>
     <row r="2091">
@@ -88338,7 +88338,7 @@
         <v>316659</v>
       </c>
       <c r="L2106">
-        <v>73.98999999999999</v>
+        <v>73.99</v>
       </c>
     </row>
     <row r="2107">
@@ -97284,7 +97284,7 @@
         <v>2111</v>
       </c>
       <c r="L2337">
-        <v>565.95</v>
+        <v>565.9500000000001</v>
       </c>
     </row>
     <row r="2338">
@@ -98894,7 +98894,7 @@
         <v>5245</v>
       </c>
       <c r="L2372">
-        <v>583.4299999999999</v>
+        <v>583.43</v>
       </c>
     </row>
     <row r="2373">
@@ -98986,7 +98986,7 @@
         <v>4962</v>
       </c>
       <c r="L2374">
-        <v>601.45</v>
+        <v>601.4500000000001</v>
       </c>
     </row>
     <row r="2375">
@@ -99216,7 +99216,7 @@
         <v>17999</v>
       </c>
       <c r="L2379">
-        <v>604.8099999999999</v>
+        <v>604.81</v>
       </c>
     </row>
     <row r="2380">
@@ -100596,7 +100596,7 @@
         <v>1203</v>
       </c>
       <c r="L2409">
-        <v>724.7</v>
+        <v>724.7000000000001</v>
       </c>
     </row>
     <row r="2410">
@@ -100734,7 +100734,7 @@
         <v>25237</v>
       </c>
       <c r="L2412">
-        <v>726.45</v>
+        <v>726.4500000000001</v>
       </c>
     </row>
     <row r="2413">
@@ -100826,7 +100826,7 @@
         <v>2584</v>
       </c>
       <c r="L2414">
-        <v>659.1799999999999</v>
+        <v>659.18</v>
       </c>
     </row>
     <row r="2415">
@@ -101332,7 +101332,7 @@
         <v>13031</v>
       </c>
       <c r="L2425">
-        <v>648.95</v>
+        <v>648.9500000000001</v>
       </c>
     </row>
     <row r="2426">
@@ -101470,7 +101470,7 @@
         <v>15155</v>
       </c>
       <c r="L2428">
-        <v>616.0599999999999</v>
+        <v>616.06</v>
       </c>
     </row>
     <row r="2429">
@@ -104083,7 +104083,7 @@
         <v>196</v>
       </c>
       <c r="L2485">
-        <v>80.98999999999999</v>
+        <v>80.99</v>
       </c>
     </row>
     <row r="2486">
@@ -107763,7 +107763,7 @@
         <v>3345</v>
       </c>
       <c r="L2565">
-        <v>67.23999999999999</v>
+        <v>67.24</v>
       </c>
     </row>
     <row r="2566">
@@ -109511,7 +109511,7 @@
         <v>517</v>
       </c>
       <c r="L2603">
-        <v>76.37</v>
+        <v>76.37000000000001</v>
       </c>
     </row>
     <row r="2604">

</xml_diff>